<commit_message>
finished data cleaning halfway
</commit_message>
<xml_diff>
--- a/data_collection.xlsx
+++ b/data_collection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\Desktop\DataScience\Projects\02_Newton_Housing_Prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\Desktop\DataScience\Projects\02_Boston_Housing_Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEB41D65-844B-40AB-8250-CFDE087539C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3D7698-3BD1-4FC1-A58C-3A0568D5C1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DD8F3E2-20EA-41B5-BF86-43A921568A69}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>East Boston</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Central</t>
-  </si>
-  <si>
-    <t>Beacon Hill/ Back Bay</t>
   </si>
   <si>
     <t>-</t>
@@ -643,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,81 +678,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8369006-583D-4E33-B969-E02034BEF822}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1067,7 @@
     <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1097,36 +1080,37 @@
       <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>33.06</v>
       </c>
       <c r="E2" s="1">
-        <f>ROUND(D2/$D$23,3)</f>
+        <f t="shared" ref="E2:E22" si="0">ROUND(D2/$D$23,3)</f>
         <v>0.10299999999999999</v>
       </c>
-      <c r="F2" s="28">
-        <f xml:space="preserve"> 1000 * E2</f>
-        <v>103</v>
-      </c>
-      <c r="G2" s="34">
+      <c r="F2" s="23">
+        <f xml:space="preserve"> ROUND(500 * E2,0)</f>
+        <v>52</v>
+      </c>
+      <c r="G2" s="28">
         <v>1288</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1137,448 +1121,464 @@
         <v>9.2899999999999991</v>
       </c>
       <c r="E3" s="1">
-        <f>ROUND(D3/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F3" s="28">
-        <f t="shared" ref="F3:F22" si="0" xml:space="preserve"> 1000 * E3</f>
-        <v>29</v>
+      <c r="F3" s="23">
+        <f t="shared" ref="F3:F22" si="1" xml:space="preserve"> ROUND(500 * E3,0)</f>
+        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>277</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="9">
         <v>29.62</v>
       </c>
       <c r="E4" s="9">
-        <f>ROUND(D4/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="F4" s="29">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="G4" s="35">
+      <c r="F4" s="24">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="G4" s="29">
         <v>2993</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="16">
+      <c r="C5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="15">
         <v>1.66</v>
       </c>
-      <c r="E5" s="16">
-        <f>ROUND(D5/$D$23,3)</f>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="F5" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G5" s="16">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>1.49</v>
       </c>
       <c r="E6" s="1">
-        <f>ROUND(D6/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F6" s="28">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="F6" s="23">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1">
         <v>3.25</v>
       </c>
       <c r="E7" s="1">
-        <f>ROUND(D7/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="F7" s="28">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="F7" s="23">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="31"/>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
         <v>0.24</v>
       </c>
       <c r="E8" s="1">
-        <f>ROUND(D8/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="F8" s="28">
-        <f xml:space="preserve"> 1000 * E8</f>
+      <c r="F8" s="23">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="32"/>
+      <c r="B9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.96</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="21">
+        <v>200</v>
+      </c>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2.09</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G10" s="12">
+        <v>266</v>
+      </c>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="F11" s="23">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2108</v>
+      </c>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="23">
-        <v>0.96</v>
-      </c>
-      <c r="E9" s="23">
-        <f>ROUND(D9/$D$23,3)</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F9" s="31">
-        <f xml:space="preserve"> 1000 * E9</f>
-        <v>3</v>
-      </c>
-      <c r="G9" s="24">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="16">
-        <v>2.09</v>
-      </c>
-      <c r="E10" s="16">
-        <f>ROUND(D10/$D$23,3)</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F10" s="30">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G10" s="17">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="23">
-        <v>3.8</v>
-      </c>
-      <c r="E11" s="23">
-        <f>ROUND(D11/$D$23,3)</f>
-        <v>1.2E-2</v>
-      </c>
-      <c r="F11" s="31">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="G11" s="36">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="12">
+      <c r="D12" s="1">
         <v>21.05</v>
       </c>
-      <c r="E12" s="12">
-        <f>ROUND(D12/$D$23,3)</f>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F12" s="32">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="G12" s="37">
+      <c r="F12" s="23">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="G12" s="28">
         <v>1051</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1">
         <v>7.24</v>
       </c>
       <c r="E13" s="1">
-        <f>ROUND(D13/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>2.3E-2</v>
       </c>
-      <c r="F13" s="28">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="G13" s="34">
+      <c r="F13" s="23">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G13" s="28">
         <v>1392</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1">
         <v>7.74</v>
       </c>
       <c r="E14" s="1">
-        <f>ROUND(D14/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
-      <c r="F14" s="28">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="G14" s="34">
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G14" s="28">
         <v>1989</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
         <v>3.36</v>
       </c>
       <c r="E15" s="1">
-        <f>ROUND(D15/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F15" s="28">
-        <f t="shared" si="0"/>
-        <v>11</v>
+      <c r="F15" s="23">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="G15" s="1">
         <v>979</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1">
         <v>26.21</v>
       </c>
       <c r="E16" s="1">
-        <f>ROUND(D16/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F16" s="28">
-        <f t="shared" si="0"/>
-        <v>82</v>
+      <c r="F16" s="23">
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="G16" s="1">
         <v>674</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1">
         <v>41.62</v>
       </c>
       <c r="E17" s="1">
-        <f>ROUND(D17/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="F17" s="28">
-        <f t="shared" si="0"/>
-        <v>130</v>
+      <c r="F17" s="23">
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="H17" s="33"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1">
         <f>17.66-0.59</f>
         <v>17.07</v>
       </c>
       <c r="E18" s="1">
-        <f>ROUND(D18/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F18" s="28">
-        <f t="shared" si="0"/>
-        <v>53</v>
+      <c r="F18" s="23">
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="G18" s="1">
         <v>847</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1">
         <v>19.350000000000001</v>
       </c>
       <c r="E19" s="1">
-        <f>ROUND(D19/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="F19" s="28">
-        <f t="shared" si="0"/>
-        <v>61</v>
+      <c r="F19" s="23">
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="G19" s="1">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1">
         <v>25.28</v>
       </c>
       <c r="E20" s="1">
-        <f>ROUND(D20/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F20" s="28">
-        <f t="shared" si="0"/>
-        <v>79</v>
+      <c r="F20" s="23">
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="G20" s="1">
         <v>134</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1">
         <v>35.36</v>
       </c>
       <c r="E21" s="1">
-        <f>ROUND(D21/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>0.111</v>
       </c>
-      <c r="F21" s="28">
-        <f t="shared" si="0"/>
-        <v>111</v>
+      <c r="F21" s="23">
+        <f t="shared" si="1"/>
+        <v>56</v>
       </c>
       <c r="G21" s="1">
         <v>172</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1">
         <v>30.01</v>
       </c>
       <c r="E22" s="1">
-        <f>ROUND(D22/$D$23,3)</f>
+        <f t="shared" si="0"/>
         <v>9.4E-2</v>
       </c>
-      <c r="F22" s="28">
-        <f t="shared" si="0"/>
-        <v>94</v>
+      <c r="F22" s="23">
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
       <c r="G22" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="33"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
@@ -1591,19 +1591,18 @@
         <f>SUM(E2:E22)</f>
         <v>1.0020000000000002</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="3">
         <f>SUM(F2:F22)</f>
-        <v>1002</v>
-      </c>
-      <c r="G23" s="34">
+        <v>508</v>
+      </c>
+      <c r="G23" s="3">
         <f>SUM(G2:G22)</f>
         <v>14705</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>